<commit_message>
Schnittstelle: Stand bis jetzt.
</commit_message>
<xml_diff>
--- a/Documents/Phasen/Concept/Schnittstelle_Server.xlsx
+++ b/Documents/Phasen/Concept/Schnittstelle_Server.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="91">
   <si>
     <t>Context Root:</t>
   </si>
@@ -119,9 +119,6 @@
   </si>
   <si>
     <t>Liefert die Rundendaten sowie alle beantworteten Fragen und die Ergebnisse beider Spieler</t>
-  </si>
-  <si>
-    <t>flag_answer</t>
   </si>
   <si>
     <t>Akzeptiert oder lehnt die Duellanfrage des Gegenspielers ab.
@@ -175,16 +172,6 @@
   <si>
     <t>Statusmeldung, ob Server-Konfiguration korrekt (ReST-WS + DB verfügbar)
 Gibt eine HTML-Seite zurück</t>
-  </si>
-  <si>
-    <t>{
- [question : {
-  // Fragenattribute
- }],
- [answer : {
-  // Antworten des Gegners
- }],
-}</t>
   </si>
   <si>
     <t>{
@@ -201,15 +188,6 @@
 }</t>
   </si>
   <si>
-    <t>[ {
- categorie_name : {
-  [question : {
-   // Fragenattribute
-  } ]
- }
-} ]</t>
-  </si>
-  <si>
     <t>user/register</t>
   </si>
   <si>
@@ -306,9 +284,6 @@
   </si>
   <si>
     <t>game/getGameOverview/{gameID}</t>
-  </si>
-  <si>
-    <t>game/getRandomCategories/{gameID}</t>
   </si>
   <si>
     <t>game/sendRoundResult</t>
@@ -390,6 +365,263 @@
   <si>
     <t>Hans Wurst</t>
   </si>
+  <si>
+    <t>flag_answer ("true"/"false")</t>
+  </si>
+  <si>
+    <t>200/404/406 (flag NOT IN ("true", "false")</t>
+  </si>
+  <si>
+    <t>game/randomCategoriesFor/{gameID}</t>
+  </si>
+  <si>
+    <t>[
+   categoryName : &lt;cat name&gt;,
+   questions : [3x questions]
+]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[{
+  "categoryName" : "Logik und Algebra",
+  "questions" : [{
+    "fragenID" : 1,
+    "kategorie_name" : "Logik und Algebra",
+    "unterkategorie_name" : "uk",
+    "flag_fragenTyp_mult" : false,
+    "frage" : "Frage 1",
+    "antwortmoeglichkeit1" : "A",
+    "antwortmoeglichkeit2" : "B",
+    "antwortmoeglichkeit3" : "C",
+    "antwortmoeglichkeit4" : "D",
+    "wahrheitAntwortmoeglichkeit1" : false,
+    "wahrheitAntwortmoeglichkeit2" : false,
+    "wahrheitAntwortmoeglichkeit3" : false,
+    "wahrheitAntwortmoeglichkeit4" : true,
+    "flag_frageValidiert" : true
+   }, {
+    "fragenID" : 2,
+    "kategorie_name" : "Logik und Algebra",
+    "unterkategorie_name" : "uk",
+    "flag_fragenTyp_mult" : false,
+    "frage" : "Frage 2",
+    "antwortmoeglichkeit1" : "A",
+    "antwortmoeglichkeit2" : "B",
+    "antwortmoeglichkeit3" : "C",
+    "antwortmoeglichkeit4" : "D",
+    "wahrheitAntwortmoeglichkeit1" : false,
+    "wahrheitAntwortmoeglichkeit2" : false,
+    "wahrheitAntwortmoeglichkeit3" : false,
+    "wahrheitAntwortmoeglichkeit4" : true,
+    "flag_frageValidiert" : true
+   }, {
+    "fragenID" : 3,
+    "kategorie_name" : "Logik und Algebra",
+    "unterkategorie_name" : "uk2",
+    "flag_fragenTyp_mult" : false,
+    "frage" : "Frage 3",
+    "antwortmoeglichkeit1" : "A",
+    "antwortmoeglichkeit2" : "B",
+    "antwortmoeglichkeit3" : "C",
+    "antwortmoeglichkeit4" : "D",
+    "wahrheitAntwortmoeglichkeit1" : false,
+    "wahrheitAntwortmoeglichkeit2" : false,
+    "wahrheitAntwortmoeglichkeit3" : false,
+    "wahrheitAntwortmoeglichkeit4" : true,
+    "flag_frageValidiert" : true
+   }
+  ]
+ }, {
+  "categoryName" : "Methoden der Wirtschaftsinformatik",
+  "questions" : [{
+    "fragenID" : 4,
+    "kategorie_name" : "Methoden der Wirtschaftsinformatik",
+    "unterkategorie_name" : "uk",
+    "flag_fragenTyp_mult" : false,
+    "frage" : "Frage 4",
+    "antwortmoeglichkeit1" : "A",
+    "antwortmoeglichkeit2" : "B",
+    "antwortmoeglichkeit3" : "C",
+    "antwortmoeglichkeit4" : "D",
+    "wahrheitAntwortmoeglichkeit1" : false,
+    "wahrheitAntwortmoeglichkeit2" : false,
+    "wahrheitAntwortmoeglichkeit3" : false,
+    "wahrheitAntwortmoeglichkeit4" : true,
+    "flag_frageValidiert" : true
+   }, {
+    "fragenID" : 5,
+    "kategorie_name" : "Methoden der Wirtschaftsinformatik",
+    "unterkategorie_name" : "uk",
+    "flag_fragenTyp_mult" : false,
+    "frage" : "Frage 5",
+    "antwortmoeglichkeit1" : "A",
+    "antwortmoeglichkeit2" : "B",
+    "antwortmoeglichkeit3" : "C",
+    "antwortmoeglichkeit4" : "D",
+    "wahrheitAntwortmoeglichkeit1" : false,
+    "wahrheitAntwortmoeglichkeit2" : false,
+    "wahrheitAntwortmoeglichkeit3" : false,
+    "wahrheitAntwortmoeglichkeit4" : true,
+    "flag_frageValidiert" : true
+   }, {
+    "fragenID" : 6,
+    "kategorie_name" : "Methoden der Wirtschaftsinformatik",
+    "unterkategorie_name" : "uk2",
+    "flag_fragenTyp_mult" : false,
+    "frage" : "Frage 6",
+    "antwortmoeglichkeit1" : "A",
+    "antwortmoeglichkeit2" : "B",
+    "antwortmoeglichkeit3" : "C",
+    "antwortmoeglichkeit4" : "D",
+    "wahrheitAntwortmoeglichkeit1" : false,
+    "wahrheitAntwortmoeglichkeit2" : false,
+    "wahrheitAntwortmoeglichkeit3" : false,
+    "wahrheitAntwortmoeglichkeit4" : true,
+    "flag_frageValidiert" : true
+   }
+  ]
+ }, {
+  "categoryName" : "Verteilte Systeme",
+  "questions" : [{
+    "fragenID" : 7,
+    "kategorie_name" : "Verteilte Systeme",
+    "unterkategorie_name" : "uk",
+    "flag_fragenTyp_mult" : false,
+    "frage" : "Frage 7",
+    "antwortmoeglichkeit1" : "A",
+    "antwortmoeglichkeit2" : "B",
+    "antwortmoeglichkeit3" : "C",
+    "antwortmoeglichkeit4" : "D",
+    "wahrheitAntwortmoeglichkeit1" : false,
+    "wahrheitAntwortmoeglichkeit2" : false,
+    "wahrheitAntwortmoeglichkeit3" : false,
+    "wahrheitAntwortmoeglichkeit4" : true,
+    "flag_frageValidiert" : true
+   }, {
+    "fragenID" : 8,
+    "kategorie_name" : "Verteilte Systeme",
+    "unterkategorie_name" : "uk",
+    "flag_fragenTyp_mult" : false,
+    "frage" : "Frage 8",
+    "antwortmoeglichkeit1" : "A",
+    "antwortmoeglichkeit2" : "B",
+    "antwortmoeglichkeit3" : "C",
+    "antwortmoeglichkeit4" : "D",
+    "wahrheitAntwortmoeglichkeit1" : false,
+    "wahrheitAntwortmoeglichkeit2" : false,
+    "wahrheitAntwortmoeglichkeit3" : false,
+    "wahrheitAntwortmoeglichkeit4" : true,
+    "flag_frageValidiert" : true
+   }, {
+    "fragenID" : 9,
+    "kategorie_name" : "Verteilte Systeme",
+    "unterkategorie_name" : "uk2",
+    "flag_fragenTyp_mult" : false,
+    "frage" : "Frage 9",
+    "antwortmoeglichkeit1" : "A",
+    "antwortmoeglichkeit2" : "B",
+    "antwortmoeglichkeit3" : "C",
+    "antwortmoeglichkeit4" : "D",
+    "wahrheitAntwortmoeglichkeit1" : false,
+    "wahrheitAntwortmoeglichkeit2" : false,
+    "wahrheitAntwortmoeglichkeit3" : false,
+    "wahrheitAntwortmoeglichkeit4" : true,
+    "flag_frageValidiert" : true
+   }
+  ]
+ }
+]
+</t>
+  </si>
+  <si>
+    <t>{
+ questions : [questions],
+ answers : [answers]
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+ "questions" : [{
+   "fragenID" : 7,
+   "kategorie_name" : "Verteilte Systeme",
+   "unterkategorie_name" : "uk",
+   "flag_fragenTyp_mult" : false,
+   "frage" : "Frage 7",
+   "antwortmoeglichkeit1" : "A",
+   "antwortmoeglichkeit2" : "B",
+   "antwortmoeglichkeit3" : "C",
+   "antwortmoeglichkeit4" : "D",
+   "wahrheitAntwortmoeglichkeit1" : false,
+   "wahrheitAntwortmoeglichkeit2" : false,
+   "wahrheitAntwortmoeglichkeit3" : false,
+   "wahrheitAntwortmoeglichkeit4" : true,
+   "flag_frageValidiert" : true
+  }, {
+   "fragenID" : 8,
+   "kategorie_name" : "Verteilte Systeme",
+   "unterkategorie_name" : "uk",
+   "flag_fragenTyp_mult" : false,
+   "frage" : "Frage 8",
+   "antwortmoeglichkeit1" : "A",
+   "antwortmoeglichkeit2" : "B",
+   "antwortmoeglichkeit3" : "C",
+   "antwortmoeglichkeit4" : "D",
+   "wahrheitAntwortmoeglichkeit1" : false,
+   "wahrheitAntwortmoeglichkeit2" : false,
+   "wahrheitAntwortmoeglichkeit3" : false,
+   "wahrheitAntwortmoeglichkeit4" : true,
+   "flag_frageValidiert" : true
+  }, {
+   "fragenID" : 9,
+   "kategorie_name" : "Verteilte Systeme",
+   "unterkategorie_name" : "uk2",
+   "flag_fragenTyp_mult" : false,
+   "frage" : "Frage 9",
+   "antwortmoeglichkeit1" : "A",
+   "antwortmoeglichkeit2" : "B",
+   "antwortmoeglichkeit3" : "C",
+   "antwortmoeglichkeit4" : "D",
+   "wahrheitAntwortmoeglichkeit1" : false,
+   "wahrheitAntwortmoeglichkeit2" : false,
+   "wahrheitAntwortmoeglichkeit3" : false,
+   "wahrheitAntwortmoeglichkeit4" : true,
+   "flag_frageValidiert" : true
+  }
+ ],
+ "answers" : [{
+   "fragenID" : 7,
+   "rundenID" : 21,
+   "benutzername" : "Kevin",
+   "antwortmoeglichkeit1_check" : false,
+   "antwortmoeglichkeit2_check" : false,
+   "antwortmoeglichkeit3_check" : false,
+   "antwortmoeglichkeit4_check" : true,
+   "flagFrageAngezeigt" : true,
+   "ergebnis_check" : true
+  }, {
+   "fragenID" : 8,
+   "rundenID" : 21,
+   "benutzername" : "Kevin",
+   "antwortmoeglichkeit1_check" : false,
+   "antwortmoeglichkeit2_check" : false,
+   "antwortmoeglichkeit3_check" : false,
+   "antwortmoeglichkeit4_check" : true,
+   "flagFrageAngezeigt" : true,
+   "ergebnis_check" : true
+  }, {
+   "fragenID" : 9,
+   "rundenID" : 21,
+   "benutzername" : "Kevin",
+   "antwortmoeglichkeit1_check" : false,
+   "antwortmoeglichkeit2_check" : false,
+   "antwortmoeglichkeit3_check" : false,
+   "antwortmoeglichkeit4_check" : true,
+   "flagFrageAngezeigt" : true,
+   "ergebnis_check" : true
+  }
+ ]
+}
+</t>
+  </si>
 </sst>
 </file>
 
@@ -447,7 +679,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -467,6 +699,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,7 +773,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="A4:O22" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="A4:O22"/>
+  <autoFilter ref="A4:O22">
+    <filterColumn colId="13">
+      <filters>
+        <filter val="nein"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="15">
     <tableColumn id="1" name="Resource" dataDxfId="14"/>
     <tableColumn id="2" name="Param1" dataDxfId="13"/>
@@ -849,8 +1090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +1112,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -891,7 +1132,7 @@
         <v>4</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>5</v>
@@ -900,7 +1141,7 @@
         <v>7</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>13</v>
@@ -912,16 +1153,16 @@
         <v>17</v>
       </c>
       <c r="M4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="O4" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -929,37 +1170,37 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="I5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="105" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>21</v>
@@ -968,7 +1209,7 @@
         <v>10</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J6" s="7"/>
       <c r="K6" s="1" t="s">
@@ -977,15 +1218,15 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -999,33 +1240,33 @@
         <v>10</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>14</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>9</v>
@@ -1034,10 +1275,10 @@
         <v>12</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>27</v>
@@ -1045,15 +1286,15 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1061,7 +1302,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>12</v>
@@ -1070,21 +1311,21 @@
         <v>200</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1092,7 +1333,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>12</v>
@@ -1101,7 +1342,7 @@
         <v>24</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>25</v>
@@ -1109,15 +1350,15 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1125,7 +1366,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>10</v>
@@ -1144,15 +1385,15 @@
       </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>20</v>
@@ -1166,10 +1407,10 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>19</v>
@@ -1177,15 +1418,15 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1193,7 +1434,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>12</v>
@@ -1202,7 +1443,7 @@
         <v>200</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>22</v>
@@ -1210,15 +1451,15 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1232,53 +1473,53 @@
         <v>12</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J14" s="7"/>
       <c r="K14" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H15" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I15" s="1"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="1" t="s">
+      <c r="I15" s="4"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="120" x14ac:dyDescent="0.25">
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1289,13 +1530,13 @@
         <v>9</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>28</v>
@@ -1305,15 +1546,15 @@
         <v>26</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="120" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1325,7 +1566,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J17" s="7"/>
       <c r="K17" s="1" t="s">
@@ -1334,15 +1575,15 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1350,7 +1591,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>12</v>
@@ -1365,18 +1606,18 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1386,25 +1627,25 @@
         <v>9</v>
       </c>
       <c r="H19" s="1"/>
-      <c r="I19" s="6">
-        <v>200</v>
+      <c r="I19" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="J19" s="7"/>
       <c r="K19" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="120" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1412,33 +1653,35 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J20" s="7"/>
+        <v>87</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>88</v>
+      </c>
       <c r="K20" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1447,30 +1690,26 @@
       <c r="G21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="6">
+        <v>200</v>
+      </c>
+      <c r="J21" s="7"/>
       <c r="K21" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="135" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1478,25 +1717,27 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J22" s="7"/>
+        <v>89</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>90</v>
+      </c>
       <c r="K22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create game now regards category intersection.
</commit_message>
<xml_diff>
--- a/Documents/Phasen/Concept/Schnittstelle_Server.xlsx
+++ b/Documents/Phasen/Concept/Schnittstelle_Server.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="89">
   <si>
     <t>Context Root:</t>
   </si>
@@ -167,9 +167,6 @@
 }</t>
   </si>
   <si>
-    <t>user/register</t>
-  </si>
-  <si>
     <t>SpringSecurity</t>
   </si>
   <si>
@@ -192,11 +189,6 @@
   </si>
   <si>
     <t>200 / 403</t>
-  </si>
-  <si>
-    <t>User
--&gt;Benutzername
--&gt;Passwort</t>
   </si>
   <si>
     <t>UserEntity
@@ -969,6 +961,18 @@
        ]
     }
 </t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>user/register/{name}</t>
+  </si>
+  <si>
+    <t>201 Spiel erstellt
+404 Spieler nicht gefunden
+409 Laufendes/Pending-Spiel mit gleichem Gegner
+406 Weniger als drei übereinstimmende Kategorien</t>
   </si>
 </sst>
 </file>
@@ -1435,8 +1439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1462,7 +1466,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
@@ -1471,7 +1475,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>9</v>
@@ -1489,7 +1493,7 @@
         <v>36</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1517,12 +1521,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>17</v>
@@ -1531,7 +1535,7 @@
         <v>6</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="1" t="s">
@@ -1548,7 +1552,7 @@
     </row>
     <row r="7" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
@@ -1558,13 +1562,13 @@
         <v>6</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -1577,10 +1581,10 @@
     </row>
     <row r="8" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
@@ -1589,13 +1593,13 @@
         <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="12"/>
@@ -1608,7 +1612,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
@@ -1627,7 +1631,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>38</v>
@@ -1635,7 +1639,7 @@
     </row>
     <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
@@ -1648,7 +1652,7 @@
         <v>20</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>21</v>
@@ -1659,12 +1663,12 @@
         <v>38</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
@@ -1695,7 +1699,7 @@
     </row>
     <row r="12" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>16</v>
@@ -1705,10 +1709,10 @@
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>15</v>
@@ -1724,7 +1728,7 @@
     </row>
     <row r="13" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
@@ -1737,7 +1741,7 @@
         <v>200</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>18</v>
@@ -1753,7 +1757,7 @@
     </row>
     <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
@@ -1763,7 +1767,7 @@
         <v>8</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="1" t="s">
@@ -1780,11 +1784,11 @@
     </row>
     <row r="15" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>8</v>
@@ -1805,20 +1809,20 @@
     </row>
     <row r="16" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>23</v>
@@ -1836,7 +1840,7 @@
     </row>
     <row r="17" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
@@ -1844,7 +1848,7 @@
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="1" t="s">
@@ -1852,7 +1856,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="9" t="s">
+      <c r="J17" s="12" t="s">
         <v>38</v>
       </c>
       <c r="K17" s="1" t="s">
@@ -1861,7 +1865,7 @@
     </row>
     <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
@@ -1871,10 +1875,10 @@
         <v>8</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>25</v>
@@ -1890,17 +1894,17 @@
     </row>
     <row r="19" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="1" t="s">
@@ -1917,7 +1921,7 @@
     </row>
     <row r="20" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
@@ -1927,10 +1931,10 @@
         <v>8</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>27</v>
@@ -1938,7 +1942,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>38</v>
@@ -1946,7 +1950,7 @@
     </row>
     <row r="21" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>28</v>
@@ -1973,7 +1977,7 @@
     </row>
     <row r="22" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
@@ -1983,10 +1987,10 @@
         <v>8</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>30</v>
@@ -1994,7 +1998,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
VerifyCredentials als Ressource mit aufgenommen.
</commit_message>
<xml_diff>
--- a/Documents/Phasen/Concept/Schnittstelle_Server.xlsx
+++ b/Documents/Phasen/Concept/Schnittstelle_Server.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="91">
   <si>
     <t>Context Root:</t>
   </si>
@@ -170,12 +170,6 @@
     <t>optional (ja)</t>
   </si>
   <si>
-    <t>user/login</t>
-  </si>
-  <si>
-    <t>Loggt einen Benutzer ein.</t>
-  </si>
-  <si>
     <t>user/logout/{username}</t>
   </si>
   <si>
@@ -183,9 +177,6 @@
   </si>
   <si>
     <t>RequestBody</t>
-  </si>
-  <si>
-    <t>200 / 403</t>
   </si>
   <si>
     <t>UserEntity
@@ -987,12 +978,21 @@
 ]
 </t>
   </si>
+  <si>
+    <t>user/verifyCredentials</t>
+  </si>
+  <si>
+    <t>200 / 403 / 404</t>
+  </si>
+  <si>
+    <t>Testet, ob der Benutzer, sofern er registriert ist, sich mit dem richtigen Passwort ausgewiesen hat.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1019,6 +1019,19 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1056,7 +1069,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1086,9 +1099,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
     <dxf>
@@ -1164,9 +1185,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1204,7 +1225,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1276,7 +1297,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1452,11 +1473,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="3" width="9.7109375" customWidth="1"/>
@@ -1479,7 +1500,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
@@ -1488,7 +1509,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>9</v>
@@ -1536,10 +1557,10 @@
     </row>
     <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>17</v>
@@ -1548,7 +1569,7 @@
         <v>6</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="1" t="s">
@@ -1563,41 +1584,39 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4" t="s">
+    <row r="7" spans="1:11" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4" t="s">
+      <c r="E7" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
@@ -1606,13 +1625,13 @@
         <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="12"/>
@@ -1625,7 +1644,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
@@ -1644,7 +1663,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>37</v>
@@ -1652,7 +1671,7 @@
     </row>
     <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
@@ -1665,7 +1684,7 @@
         <v>20</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>21</v>
@@ -1681,7 +1700,7 @@
     </row>
     <row r="11" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
@@ -1712,7 +1731,7 @@
     </row>
     <row r="12" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>16</v>
@@ -1722,10 +1741,10 @@
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>15</v>
@@ -1741,7 +1760,7 @@
     </row>
     <row r="13" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
@@ -1754,7 +1773,7 @@
         <v>200</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>18</v>
@@ -1770,7 +1789,7 @@
     </row>
     <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
@@ -1780,7 +1799,7 @@
         <v>8</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="1" t="s">
@@ -1797,11 +1816,11 @@
     </row>
     <row r="15" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>8</v>
@@ -1822,20 +1841,20 @@
     </row>
     <row r="16" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>23</v>
@@ -1853,7 +1872,7 @@
     </row>
     <row r="17" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
@@ -1861,7 +1880,7 @@
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="1" t="s">
@@ -1878,7 +1897,7 @@
     </row>
     <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
@@ -1888,10 +1907,10 @@
         <v>8</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>25</v>
@@ -1907,17 +1926,17 @@
     </row>
     <row r="19" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="1" t="s">
@@ -1934,7 +1953,7 @@
     </row>
     <row r="20" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
@@ -1944,10 +1963,10 @@
         <v>8</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>27</v>
@@ -1955,7 +1974,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>37</v>
@@ -1963,10 +1982,10 @@
     </row>
     <row r="21" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>5</v>
@@ -1990,7 +2009,7 @@
     </row>
     <row r="22" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
@@ -2000,10 +2019,10 @@
         <v>8</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>29</v>
@@ -2011,7 +2030,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>37</v>
@@ -2019,7 +2038,7 @@
     </row>
     <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
@@ -2027,7 +2046,7 @@
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="1"/>
@@ -2060,7 +2079,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2072,7 +2091,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
checkCredentials und abandon als umgesetzt markiert.
</commit_message>
<xml_diff>
--- a/Documents/Phasen/Concept/Schnittstelle_Server.xlsx
+++ b/Documents/Phasen/Concept/Schnittstelle_Server.xlsx
@@ -966,9 +966,6 @@
     <t>game/abandon/{gameId}</t>
   </si>
   <si>
-    <t>200/404</t>
-  </si>
-  <si>
     <t xml:space="preserve">[{
   spielID : spielID,
   runde : runde,
@@ -979,13 +976,18 @@
 </t>
   </si>
   <si>
-    <t>user/verifyCredentials</t>
-  </si>
-  <si>
-    <t>200 / 403 / 404</t>
-  </si>
-  <si>
     <t>Testet, ob der Benutzer, sofern er registriert ist, sich mit dem richtigen Passwort ausgewiesen hat.</t>
+  </si>
+  <si>
+    <t>user/checkCredentials</t>
+  </si>
+  <si>
+    <t>200 / 401</t>
+  </si>
+  <si>
+    <t>200 Spiel ist nun aufgegeben
+404 Spiel wurde nicht gefunden
+406 Spiel war nicht aktiv oder pending</t>
   </si>
 </sst>
 </file>
@@ -1109,7 +1111,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
     <dxf>
@@ -1185,9 +1187,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1225,7 +1227,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1297,7 +1299,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1473,16 +1475,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="3" width="9.7109375" customWidth="1"/>
     <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" customWidth="1"/>
+    <col min="5" max="5" width="36.5703125" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" customWidth="1"/>
     <col min="7" max="7" width="35.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1600,15 +1602,15 @@
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="14" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -1985,7 +1987,7 @@
         <v>73</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>5</v>
@@ -2036,7 +2038,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>85</v>
       </c>
@@ -2046,14 +2048,14 @@
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>37</v>
@@ -2079,7 +2081,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2091,7 +2093,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
addFriend: Http status aktualisiert.
</commit_message>
<xml_diff>
--- a/Documents/Phasen/Concept/Schnittstelle_Server.xlsx
+++ b/Documents/Phasen/Concept/Schnittstelle_Server.xlsx
@@ -209,9 +209,6 @@
   </si>
   <si>
     <t>settings/friends/{friend}</t>
-  </si>
-  <si>
-    <t>201/404/409</t>
   </si>
   <si>
     <t>user/search/{pattern}</t>
@@ -1003,6 +1000,11 @@
 }
 </t>
   </si>
+  <si>
+    <t>201 Freund hinzugefügt
+404 Person nicht gefunden
+409 schon befreundet oder Versuch, sich mit sich selbst zu befreunden</t>
+  </si>
 </sst>
 </file>
 
@@ -1127,7 +1129,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
     <dxf>
@@ -1203,9 +1205,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1243,7 +1245,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1315,7 +1317,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1491,11 +1493,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
@@ -1528,7 +1530,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>9</v>
@@ -1576,10 +1578,10 @@
     </row>
     <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>17</v>
@@ -1588,7 +1590,7 @@
         <v>6</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="1" t="s">
@@ -1605,7 +1607,7 @@
     </row>
     <row r="7" spans="1:11" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="12" t="s">
@@ -1615,11 +1617,11 @@
         <v>6</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
@@ -1647,10 +1649,10 @@
         <v>50</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="10"/>
@@ -1690,7 +1692,7 @@
     </row>
     <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
@@ -1703,7 +1705,7 @@
         <v>20</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>21</v>
@@ -1750,7 +1752,7 @@
     </row>
     <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>16</v>
@@ -1792,7 +1794,7 @@
         <v>200</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>18</v>
@@ -1806,7 +1808,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>54</v>
       </c>
@@ -1818,7 +1820,7 @@
         <v>8</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="1" t="s">
@@ -1860,20 +1862,20 @@
     </row>
     <row r="16" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>64</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>65</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>23</v>
@@ -1891,7 +1893,7 @@
     </row>
     <row r="17" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
@@ -1899,7 +1901,7 @@
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="1" t="s">
@@ -1916,7 +1918,7 @@
     </row>
     <row r="18" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
@@ -1926,10 +1928,10 @@
         <v>8</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>25</v>
@@ -1945,17 +1947,17 @@
     </row>
     <row r="19" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="1" t="s">
@@ -1972,7 +1974,7 @@
     </row>
     <row r="20" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
@@ -1982,10 +1984,10 @@
         <v>8</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>27</v>
@@ -2001,10 +2003,10 @@
     </row>
     <row r="21" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>5</v>
@@ -2028,7 +2030,7 @@
     </row>
     <row r="22" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
@@ -2038,10 +2040,10 @@
         <v>8</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>29</v>
@@ -2057,7 +2059,7 @@
     </row>
     <row r="23" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
@@ -2065,7 +2067,7 @@
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="1"/>
@@ -2098,7 +2100,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2110,7 +2112,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
search http status hinzugefügt.
</commit_message>
<xml_diff>
--- a/Documents/Phasen/Concept/Schnittstelle_Server.xlsx
+++ b/Documents/Phasen/Concept/Schnittstelle_Server.xlsx
@@ -76,9 +76,6 @@
   </si>
   <si>
     <t>Freund entfernen</t>
-  </si>
-  <si>
-    <t>Ergebnisliste</t>
   </si>
   <si>
     <t>Liste gefundener Mitspieler, deren Name die gesuchte Phrase enthält (like '%abc%')</t>
@@ -1071,6 +1068,10 @@
     <t>200 OK
 401 Benutzername, Pwd oder beides falsch</t>
   </si>
+  <si>
+    <t>Ergebnisliste
+200 OK</t>
+  </si>
 </sst>
 </file>
 
@@ -1193,7 +1194,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
     <dxf>
@@ -1269,9 +1270,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1309,7 +1310,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1381,7 +1382,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1558,10 +1559,10 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
@@ -1577,7 +1578,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1585,7 +1586,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
@@ -1594,7 +1595,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>9</v>
@@ -1606,46 +1607,46 @@
         <v>13</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="K4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>17</v>
@@ -1654,7 +1655,7 @@
         <v>6</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="1" t="s">
@@ -1663,18 +1664,18 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>5</v>
@@ -1683,27 +1684,27 @@
         <v>6</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
@@ -1712,30 +1713,30 @@
         <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>8</v>
@@ -1744,54 +1745,54 @@
         <v>200</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>6</v>
@@ -1810,15 +1811,15 @@
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>16</v>
@@ -1828,10 +1829,10 @@
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>15</v>
@@ -1839,19 +1840,19 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>8</v>
@@ -1860,7 +1861,7 @@
         <v>200</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>18</v>
@@ -1868,15 +1869,15 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
@@ -1886,28 +1887,28 @@
         <v>8</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>8</v>
@@ -1920,46 +1921,46 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F16" s="7" t="s">
-        <v>62</v>
-      </c>
       <c r="G16" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
@@ -1967,80 +1968,80 @@
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
@@ -2050,86 +2051,86 @@
         <v>8</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>83</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>84</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
@@ -2137,19 +2138,19 @@
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2172,7 +2173,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2184,7 +2185,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Register um 406 erweitert.
</commit_message>
<xml_diff>
--- a/Documents/Phasen/Concept/Schnittstelle_Server.xlsx
+++ b/Documents/Phasen/Concept/Schnittstelle_Server.xlsx
@@ -877,11 +877,6 @@
 </t>
   </si>
   <si>
-    <t>201 Benutzer angelegt
-409 Benutzer existiert bereits
-400 kein Passwort angegeben</t>
-  </si>
-  <si>
     <t>201 Freund hinzugefügt
 404 Person nicht gefunden
 409 schon befreundet oder Versuch, sich mit sich selbst zu befreunden</t>
@@ -1072,6 +1067,12 @@
     <t>Ergebnisliste
 200 OK</t>
   </si>
+  <si>
+    <t>201 Benutzer angelegt
+406 Benutzernamen besteht nicht aus lediglich alphanumerischen Tokens
+409 Benutzer existiert bereits
+400 kein Passwort angegeben</t>
+  </si>
 </sst>
 </file>
 
@@ -1194,7 +1195,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
     <dxf>
@@ -1270,9 +1271,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1310,7 +1311,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1382,7 +1383,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1558,11 +1559,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
@@ -1641,7 +1642,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>73</v>
       </c>
@@ -1655,7 +1656,7 @@
         <v>6</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="1" t="s">
@@ -1672,7 +1673,7 @@
     </row>
     <row r="7" spans="1:11" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>72</v>
@@ -1684,7 +1685,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="12" t="s">
@@ -1769,7 +1770,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>69</v>
@@ -1887,7 +1888,7 @@
         <v>8</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="1" t="s">
@@ -1949,7 +1950,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J16" s="10" t="s">
         <v>35</v>
@@ -2070,17 +2071,17 @@
     </row>
     <row r="21" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>83</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="1" t="s">
@@ -2088,7 +2089,7 @@
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>35</v>
@@ -2109,17 +2110,17 @@
         <v>8</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>35</v>
@@ -2144,7 +2145,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>35</v>
@@ -2173,7 +2174,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2185,7 +2186,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
getCategories, updateCategories, no use: create random, stats.
</commit_message>
<xml_diff>
--- a/Documents/Phasen/Concept/Schnittstelle_Server.xlsx
+++ b/Documents/Phasen/Concept/Schnittstelle_Server.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="94">
   <si>
     <t>Context Root:</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>Übertragt den Auswahlstatus aller Kategorien</t>
-  </si>
-  <si>
-    <t>[{kategorie_name, aktiv_flag}]</t>
   </si>
   <si>
     <t>PUT</t>
@@ -989,6 +986,57 @@
 404 Spiel wurde nicht gefunden
 406 Spiel war nicht aktiv oder pending</t>
   </si>
+  <si>
+    <t>[{kategorie_name, aktiv_flag}]
+Beispiel:
+[{
+  "kategorieName" : {
+   "name" : "IT-Management"
+  },
+  "kategorieAusgewaehltCheck" : true
+ }, {
+  "kategorieName" : {
+   "name" : "Logik und Algebra"
+  },
+  "kategorieAusgewaehltCheck" : false
+ }
+]</t>
+  </si>
+  <si>
+    <t>settings/getCategories</t>
+  </si>
+  <si>
+    <t>[{
+  "kategorieName" : {
+   "name" : "IT-Management"
+  },
+  "kategorieAusgewaehltCheck" : true
+ }, {
+  "kategorieName" : {
+   "name" : "Logik und Algebra"
+  },
+  "kategorieAusgewaehltCheck" : true
+ }, {
+  "kategorieName" : {
+   "name" : "Programmierung"
+  },
+  "kategorieAusgewaehltCheck" : true
+ }, {
+  "kategorieName" : {
+   "name" : "Projektmanagement"
+  },
+  "kategorieAusgewaehltCheck" : true
+ }, {
+  "kategorieName" : {
+   "name" : "Wissenschaftliches Arbeiten"
+  },
+  "kategorieAusgewaehltCheck" : true
+ }
+]</t>
+  </si>
+  <si>
+    <t>Liefert alle möglichen Kategorien und den Status (aktiviert/deaktiviert) des aktuell angemeldeten Nutzers zurück.</t>
+  </si>
 </sst>
 </file>
 
@@ -1039,18 +1087,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1071,7 +1113,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1091,11 +1133,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1109,6 +1148,18 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1167,8 +1218,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="A4:K23" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A4:K23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="A4:K24" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A4:K24"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Resource" dataDxfId="10"/>
     <tableColumn id="6" name="RequestBody" dataDxfId="9"/>
@@ -1473,10 +1524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1494,7 +1545,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1502,7 +1553,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
@@ -1511,7 +1562,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>9</v>
@@ -1523,55 +1574,55 @@
         <v>13</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="K4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="1" t="s">
@@ -1580,45 +1631,45 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:11" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="K7" s="14" t="s">
-        <v>37</v>
+      <c r="F7" s="14"/>
+      <c r="G7" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
@@ -1627,86 +1678,86 @@
         <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12" t="s">
-        <v>37</v>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11" t="s">
+        <v>36</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="A9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="21">
         <v>200</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>37</v>
+      <c r="F9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>6</v>
@@ -1725,28 +1776,28 @@
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>16</v>
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>90</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>15</v>
@@ -1754,316 +1805,345 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="1">
         <v>200</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>18</v>
+      <c r="F13" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>93</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="7"/>
+      <c r="E14" s="6">
+        <v>200</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="G14" s="1" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="G15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>37</v>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="4" t="s">
+    <row r="16" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>37</v>
+      <c r="E16" s="4"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="17" spans="1:11" s="17" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K17" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J16" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>81</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="F18" s="7"/>
       <c r="G18" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="1" t="s">
-        <v>37</v>
+      <c r="J18" s="11" t="s">
+        <v>36</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>67</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="F19" s="7"/>
+        <v>30</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>80</v>
+      </c>
       <c r="G19" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="C20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" s="7"/>
       <c r="G20" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>86</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="6">
-        <v>200</v>
-      </c>
-      <c r="F21" s="7"/>
+      <c r="D21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="G21" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="195" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B22" s="1"/>
+        <v>72</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="C22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>72</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="6">
+        <v>200</v>
+      </c>
+      <c r="F22" s="7"/>
       <c r="G22" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="E23" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="7"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J23">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J24">
       <formula1>"nein,ja,Mock"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>